<commit_message>
Updated name, and added Readme
</commit_message>
<xml_diff>
--- a/Experiment/RunningTime+SolutionNumber(SAT Solver).xlsx
+++ b/Experiment/RunningTime+SolutionNumber(SAT Solver).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\GitHub\Yin-Yang-SAT-Solver\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012ABD7E-9687-436B-ABA6-CD8428CBCCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9ED1DB-E352-4CFE-8B49-08A80CC912C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{786B68CC-4CCC-48FD-999D-77648639387C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{786B68CC-4CCC-48FD-999D-77648639387C}"/>
   </bookViews>
   <sheets>
     <sheet name="Number of Solutions" sheetId="1" r:id="rId1"/>
@@ -342,9 +342,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,6 +350,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -533,10 +533,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'T(1,n)'!$B$1:$U$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(1,n)'!$B$1:$U$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(1,n)'!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -576,36 +583,22 @@
                 <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'T(1,n)'!$B$2:$U$2</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(1,n)'!$B$2:$U$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(1,n)'!$B$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5.6166666666671897E-5</c:v>
                 </c:pt>
@@ -644,27 +637,6 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.25920489999999935</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.57439179999999956</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.1544019333333333</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.6930842666666632</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.8804635666666663</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13.433749999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>36.635885266666669</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>90.667480166666607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -718,10 +690,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'T(1,n)'!$B$1:$U$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(1,n)'!$B$1:$U$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(1,n)'!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -761,36 +740,22 @@
                 <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'T(1,n)'!$B$3:$U$3</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(1,n)'!$B$3:$U$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(1,n)'!$B$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5.3333333333349637E-5</c:v>
                 </c:pt>
@@ -830,9 +795,6 @@
                 <c:pt idx="12">
                   <c:v>36.256256466666663</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>171.36670049999967</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -840,176 +802,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CF4E-499C-AA26-B9AE60671551}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'T(1,n)'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Unique SAT Solver</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="1270">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'T(1,n)'!$B$1:$U$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'T(1,n)'!$B$4:$U$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>2.0686666666669366E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.9906666666660637E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.299000000001459E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0672000000000439E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.8017999999999967E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0592666666666305E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4957433333333299E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.7703166666666598E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.1548000000000009E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.23350689999999899</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.81881753333333263</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.6568906666666634</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14.158216566666601</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>60.188196166666636</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>266.19534633333268</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CF4E-499C-AA26-B9AE60671551}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1025,6 +817,179 @@
         <c:smooth val="0"/>
         <c:axId val="1431975888"/>
         <c:axId val="1431969232"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'T(1,n)'!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Unique SAT Solver</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="12700" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:prstDash val="sysDot"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="2"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="1270">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'T(1,n)'!$B$1:$U$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'T(1,n)'!$B$1:$N$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'T(1,n)'!$B$4:$U$4</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'T(1,n)'!$B$4:$N$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>2.0686666666669366E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.9906666666660637E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>6.299000000001459E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.0672000000000439E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2.8017999999999967E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5.0592666666666305E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.4957433333333299E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2.7703166666666598E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8.1548000000000009E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.23350689999999899</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.81881753333333263</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3.6568906666666634</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>14.158216566666601</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-CF4E-499C-AA26-B9AE60671551}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1431975888"/>
@@ -1506,10 +1471,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'T(2,n)'!$B$1:$L$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(2,n)'!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(2,n)'!$B$1:$H$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1531,27 +1503,22 @@
                 <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'T(2,n)'!$B$2:$L$2</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(2,n)'!$B$2:$L$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(2,n)'!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6.3936666666656629E-4</c:v>
                 </c:pt>
@@ -1572,18 +1539,6 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.60939636666666608</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.0887958333333301</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.1073683999999959</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>22.174428133333333</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>104.819255133333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1637,10 +1592,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'T(2,n)'!$B$1:$L$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(2,n)'!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(2,n)'!$B$1:$H$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1662,27 +1624,22 @@
                 <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'T(2,n)'!$B$3:$L$3</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(2,n)'!$B$3:$L$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(2,n)'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.79900000000014E-4</c:v>
                 </c:pt>
@@ -1714,128 +1671,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'T(2,n)'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Unique SAT Solver</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="1270">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'T(2,n)'!$B$1:$L$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'T(2,n)'!$B$4:$L$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>8.8486666666664961E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.2325000000000036E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.7165000000000063E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.7487233333333236E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.139901733333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1381403999999968</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.402950566666632</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>106.166562633333</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F880-487E-AC55-4753CE568635}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1848,6 +1683,143 @@
         <c:smooth val="0"/>
         <c:axId val="1431975888"/>
         <c:axId val="1431969232"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'T(2,n)'!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Unique SAT Solver</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="12700" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:prstDash val="sysDot"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="2"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="1270">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'T(2,n)'!$B$1:$L$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'T(2,n)'!$B$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'T(2,n)'!$B$4:$L$4</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'T(2,n)'!$B$4:$H$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>8.8486666666664961E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.2325000000000036E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.7165000000000063E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2.7487233333333236E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.139901733333333</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.1381403999999968</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>10.402950566666632</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-F880-487E-AC55-4753CE568635}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1431975888"/>
@@ -2329,10 +2301,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'T(3,n)'!$B$1:$H$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(3,n)'!$B$1:$H$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(3,n)'!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2345,24 +2324,22 @@
                 <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'T(3,n)'!$B$2:$H$2</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(3,n)'!$B$2:$H$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(3,n)'!$B$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7.6818000000000658E-3</c:v>
                 </c:pt>
@@ -2374,15 +2351,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.05867893333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.9377166333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>38.5624015</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>397.93158736666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2436,10 +2404,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'T(3,n)'!$B$1:$H$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(3,n)'!$B$1:$H$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(3,n)'!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2452,24 +2427,22 @@
                 <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'T(3,n)'!$B$3:$H$3</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'T(3,n)'!$B$3:$H$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'T(3,n)'!$B$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2.2220333333333269E-2</c:v>
                 </c:pt>
@@ -2492,104 +2465,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'T(3,n)'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Unique SAT Solver</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="1270">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'T(3,n)'!$B$1:$H$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'T(3,n)'!$B$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.4741366666666632E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.119860866666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.81055723333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42.341274499999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-75B4-4541-916D-1A3050688A5C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2602,6 +2477,125 @@
         <c:smooth val="0"/>
         <c:axId val="1431975888"/>
         <c:axId val="1431969232"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'T(3,n)'!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Unique SAT Solver</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="12700" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:prstDash val="sysDot"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="2"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="1270">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'T(3,n)'!$B$1:$H$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'T(3,n)'!$B$1:$E$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'T(3,n)'!$B$4:$H$4</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'T(3,n)'!$B$4:$E$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1.4741366666666632E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.119860866666666</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.81055723333333</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>42.341274499999997</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-75B4-4541-916D-1A3050688A5C}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1431975888"/>
@@ -5847,7 +5841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994536F1-51AE-4898-86E3-1F56E77BFE33}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -6696,194 +6690,194 @@
         <v>0</v>
       </c>
       <c r="B1" s="37"/>
-      <c r="C1" s="33">
+      <c r="C1" s="32">
         <v>1</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="33">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="32">
         <f>C1+1</f>
         <v>2</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="33">
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="32">
         <f>G1+1</f>
         <v>3</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="33">
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="32">
         <f>K1+1</f>
         <v>4</v>
       </c>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="33">
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="32">
         <f>O1+1</f>
         <v>5</v>
       </c>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="33">
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="32">
         <f>S1+1</f>
         <v>6</v>
       </c>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="33">
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="32">
         <f>W1+1</f>
         <v>7</v>
       </c>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="33">
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="32">
         <f>AA1+1</f>
         <v>8</v>
       </c>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="33">
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="32">
         <f>AE1+1</f>
         <v>9</v>
       </c>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="33">
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="32">
         <f>AI1+1</f>
         <v>10</v>
       </c>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="35"/>
-      <c r="AQ1" s="33">
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="34"/>
+      <c r="AQ1" s="32">
         <f>AM1+1</f>
         <v>11</v>
       </c>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="35"/>
-      <c r="AU1" s="33">
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="34"/>
+      <c r="AU1" s="32">
         <f>AQ1+1</f>
         <v>12</v>
       </c>
-      <c r="AV1" s="34"/>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="33">
+      <c r="AV1" s="33"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="34"/>
+      <c r="AY1" s="32">
         <f>AU1+1</f>
         <v>13</v>
       </c>
-      <c r="AZ1" s="34"/>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="35"/>
-      <c r="BC1" s="33">
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="32">
         <f>AY1+1</f>
         <v>14</v>
       </c>
-      <c r="BD1" s="34"/>
-      <c r="BE1" s="34"/>
-      <c r="BF1" s="35"/>
-      <c r="BG1" s="33">
+      <c r="BD1" s="33"/>
+      <c r="BE1" s="33"/>
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="32">
         <f>BC1+1</f>
         <v>15</v>
       </c>
-      <c r="BH1" s="34"/>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="35"/>
-      <c r="BK1" s="33">
+      <c r="BH1" s="33"/>
+      <c r="BI1" s="33"/>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="32">
         <f>BG1+1</f>
         <v>16</v>
       </c>
-      <c r="BL1" s="34"/>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="35"/>
-      <c r="BO1" s="33">
+      <c r="BL1" s="33"/>
+      <c r="BM1" s="33"/>
+      <c r="BN1" s="34"/>
+      <c r="BO1" s="32">
         <f>BK1+1</f>
         <v>17</v>
       </c>
-      <c r="BP1" s="34"/>
-      <c r="BQ1" s="34"/>
-      <c r="BR1" s="35"/>
-      <c r="BS1" s="33">
+      <c r="BP1" s="33"/>
+      <c r="BQ1" s="33"/>
+      <c r="BR1" s="34"/>
+      <c r="BS1" s="32">
         <f>BO1+1</f>
         <v>18</v>
       </c>
-      <c r="BT1" s="34"/>
-      <c r="BU1" s="34"/>
-      <c r="BV1" s="35"/>
-      <c r="BW1" s="33">
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="33"/>
+      <c r="BV1" s="34"/>
+      <c r="BW1" s="32">
         <f>BS1+1</f>
         <v>19</v>
       </c>
-      <c r="BX1" s="34"/>
-      <c r="BY1" s="34"/>
-      <c r="BZ1" s="35"/>
-      <c r="CA1" s="33">
+      <c r="BX1" s="33"/>
+      <c r="BY1" s="33"/>
+      <c r="BZ1" s="34"/>
+      <c r="CA1" s="32">
         <f>BW1+1</f>
         <v>20</v>
       </c>
-      <c r="CB1" s="34"/>
-      <c r="CC1" s="34"/>
-      <c r="CD1" s="35"/>
-      <c r="CE1" s="33">
+      <c r="CB1" s="33"/>
+      <c r="CC1" s="33"/>
+      <c r="CD1" s="34"/>
+      <c r="CE1" s="32">
         <f>CA1+1</f>
         <v>21</v>
       </c>
-      <c r="CF1" s="34"/>
-      <c r="CG1" s="34"/>
-      <c r="CH1" s="35"/>
-      <c r="CI1" s="33">
+      <c r="CF1" s="33"/>
+      <c r="CG1" s="33"/>
+      <c r="CH1" s="34"/>
+      <c r="CI1" s="32">
         <f>CE1+1</f>
         <v>22</v>
       </c>
-      <c r="CJ1" s="34"/>
-      <c r="CK1" s="34"/>
-      <c r="CL1" s="35"/>
-      <c r="CM1" s="33">
+      <c r="CJ1" s="33"/>
+      <c r="CK1" s="33"/>
+      <c r="CL1" s="34"/>
+      <c r="CM1" s="32">
         <f>CI1+1</f>
         <v>23</v>
       </c>
-      <c r="CN1" s="34"/>
-      <c r="CO1" s="34"/>
-      <c r="CP1" s="35"/>
-      <c r="CQ1" s="33">
+      <c r="CN1" s="33"/>
+      <c r="CO1" s="33"/>
+      <c r="CP1" s="34"/>
+      <c r="CQ1" s="32">
         <f>CM1+1</f>
         <v>24</v>
       </c>
-      <c r="CR1" s="34"/>
-      <c r="CS1" s="34"/>
-      <c r="CT1" s="35"/>
-      <c r="CU1" s="33">
+      <c r="CR1" s="33"/>
+      <c r="CS1" s="33"/>
+      <c r="CT1" s="34"/>
+      <c r="CU1" s="32">
         <f>CQ1+1</f>
         <v>25</v>
       </c>
-      <c r="CV1" s="34"/>
-      <c r="CW1" s="34"/>
-      <c r="CX1" s="35"/>
-      <c r="CY1" s="33">
+      <c r="CV1" s="33"/>
+      <c r="CW1" s="33"/>
+      <c r="CX1" s="34"/>
+      <c r="CY1" s="32">
         <f>CU1+1</f>
         <v>26</v>
       </c>
-      <c r="CZ1" s="34"/>
-      <c r="DA1" s="34"/>
-      <c r="DB1" s="35"/>
-      <c r="DC1" s="33">
+      <c r="CZ1" s="33"/>
+      <c r="DA1" s="33"/>
+      <c r="DB1" s="34"/>
+      <c r="DC1" s="32">
         <f>CY1+1</f>
         <v>27</v>
       </c>
-      <c r="DD1" s="34"/>
-      <c r="DE1" s="34"/>
-      <c r="DF1" s="35"/>
+      <c r="DD1" s="33"/>
+      <c r="DE1" s="33"/>
+      <c r="DF1" s="34"/>
     </row>
     <row r="2" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A2" s="38"/>
@@ -7214,7 +7208,7 @@
       </c>
     </row>
     <row r="3" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -7513,7 +7507,7 @@
       <c r="DF3" s="11"/>
     </row>
     <row r="4" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -7723,7 +7717,7 @@
       <c r="DF4" s="12"/>
     </row>
     <row r="5" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -7900,7 +7894,7 @@
       <c r="DF5" s="12"/>
     </row>
     <row r="6" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -8044,7 +8038,7 @@
       <c r="DF6" s="12"/>
     </row>
     <row r="7" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -8211,7 +8205,7 @@
       <c r="DF7" s="13"/>
     </row>
     <row r="8" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1">
@@ -8474,7 +8468,7 @@
       <c r="DF8" s="11"/>
     </row>
     <row r="9" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -8655,7 +8649,7 @@
       <c r="DF9" s="12"/>
     </row>
     <row r="10" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="1">
         <v>3</v>
       </c>
@@ -8808,7 +8802,7 @@
       <c r="DF10" s="12"/>
     </row>
     <row r="11" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -8936,7 +8930,7 @@
       <c r="DF11" s="12"/>
     </row>
     <row r="12" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="1">
         <v>5</v>
       </c>
@@ -9101,7 +9095,7 @@
       <c r="DF12" s="13"/>
     </row>
     <row r="13" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1">
@@ -9370,7 +9364,7 @@
       <c r="DF13" s="14"/>
     </row>
     <row r="14" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="1">
         <v>2</v>
       </c>
@@ -9556,7 +9550,7 @@
       <c r="DF14" s="12"/>
     </row>
     <row r="15" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="1">
         <v>3</v>
       </c>
@@ -9709,7 +9703,7 @@
       <c r="DF15" s="12"/>
     </row>
     <row r="16" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="1">
         <v>4</v>
       </c>
@@ -9845,7 +9839,7 @@
       <c r="DF16" s="12"/>
     </row>
     <row r="17" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="1">
         <v>5</v>
       </c>
@@ -10011,6 +10005,26 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="AA1:AD1"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="AQ1:AT1"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="BG1:BJ1"/>
+    <mergeCell ref="BK1:BN1"/>
     <mergeCell ref="DC1:DF1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
@@ -10022,26 +10036,6 @@
     <mergeCell ref="CI1:CL1"/>
     <mergeCell ref="CM1:CP1"/>
     <mergeCell ref="CQ1:CT1"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="BG1:BJ1"/>
-    <mergeCell ref="BK1:BN1"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A3:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10052,7 +10046,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10378,7 +10372,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10570,8 +10564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFF2C2F-8B5A-494F-8116-5199FDA899C3}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>